<commit_message>
OOP Failed students updated
</commit_message>
<xml_diff>
--- a/assets/results.xlsx
+++ b/assets/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shani\Documents\GitHub\marks\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E954AC-D1A5-4471-B706-29554F1A5171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D144FBC4-061F-4756-8EFD-F388BFA4B732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="699">
   <si>
     <t>Sr.
 No.</t>
@@ -3473,6 +3473,9 @@
   </si>
   <si>
     <t>NC</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -10459,8 +10462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11020,7 +11023,9 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>698</v>
+      </c>
       <c r="H12" s="8">
         <v>79</v>
       </c>
@@ -11067,7 +11072,9 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>698</v>
+      </c>
       <c r="H13" s="8">
         <v>71</v>
       </c>
@@ -11161,7 +11168,9 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>698</v>
+      </c>
       <c r="H15" s="8">
         <v>77</v>
       </c>
@@ -11255,7 +11264,9 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>698</v>
+      </c>
       <c r="H17" s="8">
         <v>68</v>
       </c>
@@ -11349,7 +11360,9 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>698</v>
+      </c>
       <c r="H19" s="8">
         <v>71</v>
       </c>
@@ -18745,7 +18758,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" ref="L35:L66" si="2">SUM(D35:K35)</f>
+        <f t="shared" ref="L35:L52" si="2">SUM(D35:K35)</f>
         <v>0</v>
       </c>
       <c r="M35" s="1">
@@ -21015,7 +21028,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" ref="I35:I66" si="2">SUM(D35:H35)</f>
+        <f t="shared" ref="I35:I52" si="2">SUM(D35:H35)</f>
         <v>0</v>
       </c>
       <c r="J35" s="1">

</xml_diff>